<commit_message>
fixed step increases in catch data
</commit_message>
<xml_diff>
--- a/Data/table_2.xlsx
+++ b/Data/table_2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jepa88/GitHub/northsea_mpa_sust_fish/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D2DE46B-7DA0-CC43-A94B-1668583987C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9066FEB-4ACD-0645-AE62-AF81AAC36D95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15220" yWindow="-21600" windowWidth="19200" windowHeight="21600" activeTab="2" xr2:uid="{6C9829FD-DC47-9042-ABCE-AB11A61A76C3}"/>
+    <workbookView xWindow="15340" yWindow="-21600" windowWidth="19080" windowHeight="21600" activeTab="2" xr2:uid="{6C9829FD-DC47-9042-ABCE-AB11A61A76C3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -84,6 +84,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -120,9 +123,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2941,11 +2946,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BD2CD9A-A721-D945-9D79-610CBB630589}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:G63"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E64" sqref="E64"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2973,7 +2977,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2991,11 +2995,11 @@
         <v>0.5</v>
       </c>
       <c r="G2">
-        <f>E2</f>
-        <v>-1.6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+        <f>E2-E4</f>
+        <v>-0.53333333333333344</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -3017,7 +3021,7 @@
         <v>-0.64999999999999991</v>
       </c>
     </row>
-    <row r="4" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -3035,11 +3039,11 @@
         <v>0.5</v>
       </c>
       <c r="G4">
-        <f>E4-E3</f>
-        <v>1.1833333333333333</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+        <f>E4</f>
+        <v>-1.0666666666666667</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -3057,11 +3061,11 @@
         <v>0.75</v>
       </c>
       <c r="G5">
-        <f>E5</f>
-        <v>-3.375</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+        <f>E5-E7</f>
+        <v>-0.97499999999999964</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -3079,11 +3083,11 @@
         <v>0.75</v>
       </c>
       <c r="G6">
-        <f>E6-E5</f>
-        <v>1.7749999999999999</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+        <f>E6</f>
+        <v>-1.6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -3105,7 +3109,7 @@
         <v>-0.80000000000000027</v>
       </c>
     </row>
-    <row r="8" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -3127,7 +3131,7 @@
         <v>-2.1333333333333333</v>
       </c>
     </row>
-    <row r="9" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -3148,7 +3152,7 @@
         <v>-1.0666666666666669</v>
       </c>
     </row>
-    <row r="10" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -3169,7 +3173,7 @@
         <v>-1.2999999999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -3191,7 +3195,7 @@
         <v>4.1333333333333329</v>
       </c>
     </row>
-    <row r="12" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>5</v>
       </c>
@@ -3212,7 +3216,7 @@
         <v>2.0666666666666673</v>
       </c>
     </row>
-    <row r="13" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>5</v>
       </c>
@@ -3233,7 +3237,7 @@
         <v>3.8999999999999995</v>
       </c>
     </row>
-    <row r="14" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>5</v>
       </c>
@@ -3244,40 +3248,40 @@
         <v>30</v>
       </c>
       <c r="E14">
-        <f ca="1">($D$22/$D$17)*$E$16*F14</f>
+        <f>($D$14/$D$19)*$E$19*F14</f>
         <v>-5.4</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="3">
         <v>1</v>
       </c>
       <c r="G14">
-        <f ca="1">E14</f>
-        <v>-0.9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+        <f>E14-E16</f>
+        <v>-2.7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>5</v>
       </c>
       <c r="C15" t="s">
         <v>7</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="3">
         <v>30</v>
       </c>
-      <c r="E15">
-        <f ca="1">($D$22/$D$17)*$E$16*F15</f>
+      <c r="E15" s="3">
+        <f>(D15/D19)*E19*F15</f>
         <v>-4.0500000000000007</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="3">
         <v>0.75</v>
       </c>
       <c r="G15">
-        <f t="shared" ref="G15:G31" ca="1" si="0">E15</f>
-        <v>-1.35</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+        <f>E15-E18</f>
+        <v>-2.0250000000000004</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>5</v>
       </c>
@@ -3288,18 +3292,18 @@
         <v>15</v>
       </c>
       <c r="E16">
-        <f ca="1">($D$18/$D$17)*$E$16*F16</f>
+        <f>($D$16/$D$19)*$E$19*F16</f>
         <v>-2.7</v>
       </c>
-      <c r="F16">
-        <v>1</v>
-      </c>
-      <c r="G16">
-        <f t="shared" ca="1" si="0"/>
-        <v>-1.8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="F16" s="3">
+        <v>1</v>
+      </c>
+      <c r="G16" s="2">
+        <f>E16-E19</f>
+        <v>-0.90000000000000013</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>5</v>
       </c>
@@ -3310,83 +3314,83 @@
         <v>30</v>
       </c>
       <c r="E17">
-        <f ca="1">($D$22/$D$17)*$E$16*F17</f>
+        <f>E22*3</f>
         <v>-2.7</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="3">
         <v>0.5</v>
       </c>
       <c r="G17">
-        <f t="shared" ca="1" si="0"/>
-        <v>3.8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+        <f>E17-E21</f>
+        <v>-1.35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>5</v>
       </c>
       <c r="C18" t="s">
         <v>7</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="3">
         <v>15</v>
       </c>
-      <c r="E18">
-        <f ca="1">($D$18/$D$17)*$E$16*F18</f>
+      <c r="E18" s="3">
+        <f>(D18/D20)*E19*F18</f>
         <v>-2.0250000000000004</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="3">
         <v>0.75</v>
       </c>
       <c r="G18">
-        <f t="shared" ca="1" si="0"/>
+        <f>E18-E21</f>
+        <v>-0.67500000000000027</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" s="3">
+        <v>10</v>
+      </c>
+      <c r="E19" s="3">
+        <v>-1.8</v>
+      </c>
+      <c r="F19" s="3">
+        <v>1</v>
+      </c>
+      <c r="G19" s="3">
+        <f>E19</f>
+        <v>-1.8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="3">
+        <v>10</v>
+      </c>
+      <c r="E20" s="3">
+        <f>$E$19*F20</f>
         <v>-1.35</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19" t="s">
-        <v>7</v>
-      </c>
-      <c r="D19">
-        <v>10</v>
-      </c>
-      <c r="E19">
-        <v>-1.8</v>
-      </c>
-      <c r="F19">
-        <v>1</v>
-      </c>
-      <c r="G19">
-        <f t="shared" si="0"/>
-        <v>-1.8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>5</v>
-      </c>
-      <c r="C20" t="s">
-        <v>7</v>
-      </c>
-      <c r="D20">
-        <v>10</v>
-      </c>
-      <c r="E20">
-        <f ca="1">$E$16*F20</f>
-        <v>-1.35</v>
-      </c>
-      <c r="F20">
+      <c r="F20" s="3">
         <v>0.75</v>
       </c>
       <c r="G20">
-        <f t="shared" ca="1" si="0"/>
-        <v>-2.7</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+        <f>-E20</f>
+        <v>1.35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>5</v>
       </c>
@@ -3397,18 +3401,18 @@
         <v>15</v>
       </c>
       <c r="E21">
-        <f ca="1">($D$18/$D$17)*$E$16*F21</f>
+        <f>E22*1.5</f>
         <v>-1.35</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="3">
         <v>0.5</v>
       </c>
       <c r="G21">
-        <f t="shared" ca="1" si="0"/>
-        <v>5.6999999999999993</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+        <f>E21-E22</f>
+        <v>-0.45000000000000007</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>5</v>
       </c>
@@ -3419,18 +3423,18 @@
         <v>10</v>
       </c>
       <c r="E22">
-        <f ca="1">$E$16*F22</f>
+        <f>$E$19*F22</f>
         <v>-0.9</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="3">
         <v>0.5</v>
       </c>
       <c r="G22">
-        <f t="shared" ca="1" si="0"/>
-        <v>-2.7</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+        <f t="shared" ref="G15:G31" si="0">E22</f>
+        <v>-0.9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>5</v>
       </c>
@@ -3451,7 +3455,7 @@
         <v>3.8</v>
       </c>
     </row>
-    <row r="24" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>5</v>
       </c>
@@ -3462,18 +3466,18 @@
         <v>15</v>
       </c>
       <c r="E24">
-        <f>3.8*(D24/$D$17)</f>
-        <v>1.9</v>
+        <f>3.8*1.5</f>
+        <v>5.6999999999999993</v>
       </c>
       <c r="F24">
         <v>1.5</v>
       </c>
       <c r="G24">
-        <f t="shared" si="0"/>
-        <v>1.9</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+        <f>E24-E23</f>
+        <v>1.8999999999999995</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>5</v>
       </c>
@@ -3484,18 +3488,18 @@
         <v>30</v>
       </c>
       <c r="E25">
-        <f>3.8*(D25/$D$17)</f>
-        <v>3.8</v>
+        <f>3.8*3</f>
+        <v>11.399999999999999</v>
       </c>
       <c r="F25">
         <v>1.5</v>
       </c>
       <c r="G25">
-        <f t="shared" si="0"/>
-        <v>3.8</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+        <f>E25-E24</f>
+        <v>5.6999999999999993</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>8</v>
       </c>
@@ -3512,11 +3516,11 @@
         <v>0.5</v>
       </c>
       <c r="G26">
-        <f t="shared" si="0"/>
+        <f>E26</f>
         <v>-24.6</v>
       </c>
     </row>
-    <row r="27" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>8</v>
       </c>
@@ -3533,11 +3537,11 @@
         <v>0.75</v>
       </c>
       <c r="G27">
-        <f>E26-E27</f>
-        <v>-18.200000000000003</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+        <f>E27</f>
+        <v>-6.4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>8</v>
       </c>
@@ -3554,11 +3558,11 @@
         <v>1.5</v>
       </c>
       <c r="G28">
-        <f>E27-E28*-1</f>
-        <v>-39.1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+        <f>E28</f>
+        <v>-32.700000000000003</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>8</v>
       </c>
@@ -3575,11 +3579,11 @@
         <v>0.5</v>
       </c>
       <c r="G29">
-        <f t="shared" si="0"/>
+        <f>E29</f>
         <v>-25</v>
       </c>
     </row>
-    <row r="30" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>8</v>
       </c>
@@ -3596,11 +3600,11 @@
         <v>0.75</v>
       </c>
       <c r="G30">
-        <f t="shared" si="0"/>
+        <f>E30</f>
         <v>-6.6</v>
       </c>
     </row>
-    <row r="31" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>8</v>
       </c>
@@ -3617,7 +3621,7 @@
         <v>1.5</v>
       </c>
       <c r="G31">
-        <f t="shared" si="0"/>
+        <f>E31</f>
         <v>-32.200000000000003</v>
       </c>
     </row>
@@ -3638,7 +3642,8 @@
         <v>1</v>
       </c>
       <c r="G32">
-        <v>-9.6</v>
+        <f>E32</f>
+        <v>-8.1999999999999993</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
@@ -3659,7 +3664,8 @@
         <v>1</v>
       </c>
       <c r="G33">
-        <v>-9.6</v>
+        <f>E33-E32</f>
+        <v>-8.1999999999999993</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
@@ -3680,7 +3686,8 @@
         <v>1</v>
       </c>
       <c r="G34">
-        <v>-9.6</v>
+        <f t="shared" ref="G34:G35" si="1">E34-E33</f>
+        <v>-8.1999999999999993</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
@@ -3701,7 +3708,8 @@
         <v>1</v>
       </c>
       <c r="G35">
-        <v>-9.6</v>
+        <f t="shared" si="1"/>
+        <v>-8.1999999999999993</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
@@ -3808,7 +3816,8 @@
         <v>0.75</v>
       </c>
       <c r="G40">
-        <v>-12.6</v>
+        <f>E40</f>
+        <v>-7.6</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
@@ -3829,7 +3838,8 @@
         <v>0.75</v>
       </c>
       <c r="G41">
-        <v>-12.6</v>
+        <f>E41-E40</f>
+        <v>-7.6</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
@@ -3850,7 +3860,8 @@
         <v>0.75</v>
       </c>
       <c r="G42">
-        <v>-12.6</v>
+        <f t="shared" ref="G42:G43" si="2">E42-E41</f>
+        <v>-7.5999999999999979</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
@@ -3871,7 +3882,8 @@
         <v>0.75</v>
       </c>
       <c r="G43">
-        <v>-12.6</v>
+        <f t="shared" si="2"/>
+        <v>-7.6000000000000014</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
@@ -3892,7 +3904,8 @@
         <v>1.5</v>
       </c>
       <c r="G44">
-        <v>-4.7</v>
+        <f>E44</f>
+        <v>-6.1</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
@@ -3914,7 +3927,8 @@
         <v>1.5</v>
       </c>
       <c r="G45">
-        <v>-4.7</v>
+        <f>E45-E44</f>
+        <v>-6.1</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
@@ -3936,7 +3950,8 @@
         <v>1.5</v>
       </c>
       <c r="G46">
-        <v>-4.7</v>
+        <f t="shared" ref="G46:G47" si="3">E46-E45</f>
+        <v>-6.0999999999999979</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
@@ -3958,10 +3973,11 @@
         <v>1.5</v>
       </c>
       <c r="G47">
-        <v>-4.7</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>-6.1000000000000014</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>10</v>
       </c>
@@ -3972,16 +3988,18 @@
         <v>7</v>
       </c>
       <c r="E48">
+        <f>-8.2*B48</f>
         <v>-8.1999999999999993</v>
       </c>
       <c r="F48">
         <v>1</v>
       </c>
       <c r="G48">
-        <v>-9.9</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+        <f>E48</f>
+        <v>-8.1999999999999993</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>10</v>
       </c>
@@ -3992,16 +4010,18 @@
         <v>7</v>
       </c>
       <c r="E49">
+        <f t="shared" ref="E49:E51" si="4">-8.2*B49</f>
+        <v>-16.399999999999999</v>
+      </c>
+      <c r="F49">
+        <v>1</v>
+      </c>
+      <c r="G49">
+        <f>E49-E48</f>
         <v>-8.1999999999999993</v>
       </c>
-      <c r="F49">
-        <v>1</v>
-      </c>
-      <c r="G49">
-        <v>-9.9</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>10</v>
       </c>
@@ -4012,16 +4032,18 @@
         <v>7</v>
       </c>
       <c r="E50">
+        <f t="shared" si="4"/>
+        <v>-24.599999999999998</v>
+      </c>
+      <c r="F50">
+        <v>1</v>
+      </c>
+      <c r="G50">
+        <f>E50-E49</f>
         <v>-8.1999999999999993</v>
       </c>
-      <c r="F50">
-        <v>1</v>
-      </c>
-      <c r="G50">
-        <v>-9.9</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>10</v>
       </c>
@@ -4032,16 +4054,18 @@
         <v>7</v>
       </c>
       <c r="E51">
+        <f t="shared" si="4"/>
+        <v>-32.799999999999997</v>
+      </c>
+      <c r="F51">
+        <v>1</v>
+      </c>
+      <c r="G51">
+        <f>E51-E50</f>
         <v>-8.1999999999999993</v>
       </c>
-      <c r="F51">
-        <v>1</v>
-      </c>
-      <c r="G51">
-        <v>-9.9</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>10</v>
       </c>
@@ -4052,16 +4076,18 @@
         <v>7</v>
       </c>
       <c r="E52">
+        <f>-6.3*B52</f>
         <v>-6.3</v>
       </c>
       <c r="F52">
         <v>0.5</v>
       </c>
       <c r="G52">
-        <v>-15.1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+        <f>E52</f>
+        <v>-6.3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>10</v>
       </c>
@@ -4072,16 +4098,18 @@
         <v>7</v>
       </c>
       <c r="E53">
+        <f t="shared" ref="E53:E55" si="5">-6.3*B53</f>
+        <v>-12.6</v>
+      </c>
+      <c r="F53">
+        <v>0.5</v>
+      </c>
+      <c r="G53">
+        <f>E53-E52</f>
         <v>-6.3</v>
       </c>
-      <c r="F53">
-        <v>0.5</v>
-      </c>
-      <c r="G53">
-        <v>-15.1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>10</v>
       </c>
@@ -4092,16 +4120,18 @@
         <v>7</v>
       </c>
       <c r="E54">
-        <v>-6.3</v>
+        <f t="shared" si="5"/>
+        <v>-18.899999999999999</v>
       </c>
       <c r="F54">
         <v>0.5</v>
       </c>
       <c r="G54">
-        <v>-15.1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+        <f>E54-E53</f>
+        <v>-6.2999999999999989</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>10</v>
       </c>
@@ -4112,16 +4142,18 @@
         <v>7</v>
       </c>
       <c r="E55">
-        <v>-6.3</v>
+        <f t="shared" si="5"/>
+        <v>-25.2</v>
       </c>
       <c r="F55">
         <v>0.5</v>
       </c>
       <c r="G55">
-        <v>-15.1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+        <f>E55-E54</f>
+        <v>-6.3000000000000007</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>10</v>
       </c>
@@ -4132,16 +4164,18 @@
         <v>7</v>
       </c>
       <c r="E56">
+        <f>-7.7*B56</f>
         <v>-7.7</v>
       </c>
       <c r="F56">
         <v>0.75</v>
       </c>
       <c r="G56">
-        <v>-13</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+        <f>E56</f>
+        <v>-7.7</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>10</v>
       </c>
@@ -4152,16 +4186,18 @@
         <v>7</v>
       </c>
       <c r="E57">
+        <f t="shared" ref="E57:E59" si="6">-7.7*B57</f>
+        <v>-15.4</v>
+      </c>
+      <c r="F57">
+        <v>0.75</v>
+      </c>
+      <c r="G57">
+        <f>E57-E56</f>
         <v>-7.7</v>
       </c>
-      <c r="F57">
-        <v>0.75</v>
-      </c>
-      <c r="G57">
-        <v>-13</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>10</v>
       </c>
@@ -4172,16 +4208,18 @@
         <v>7</v>
       </c>
       <c r="E58">
-        <v>-7.7</v>
+        <f t="shared" si="6"/>
+        <v>-23.1</v>
       </c>
       <c r="F58">
         <v>0.75</v>
       </c>
       <c r="G58">
-        <v>-13</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+        <f>E58-E57</f>
+        <v>-7.7000000000000011</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>10</v>
       </c>
@@ -4192,16 +4230,18 @@
         <v>7</v>
       </c>
       <c r="E59">
-        <v>-7.7</v>
+        <f t="shared" si="6"/>
+        <v>-30.8</v>
       </c>
       <c r="F59">
         <v>0.75</v>
       </c>
       <c r="G59">
-        <v>-13</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+        <f>E59-E58</f>
+        <v>-7.6999999999999993</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>10</v>
       </c>
@@ -4213,16 +4253,18 @@
       </c>
       <c r="D60" s="1"/>
       <c r="E60">
+        <f>-6.1*B60</f>
         <v>-6.1</v>
       </c>
       <c r="F60" s="1">
         <v>1.5</v>
       </c>
       <c r="G60">
-        <v>-4.7</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+        <f>E60</f>
+        <v>-6.1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>10</v>
       </c>
@@ -4234,16 +4276,18 @@
       </c>
       <c r="D61" s="1"/>
       <c r="E61">
+        <f t="shared" ref="E61:E63" si="7">-6.1*B61</f>
+        <v>-12.2</v>
+      </c>
+      <c r="F61" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="G61">
+        <f>E61-E60</f>
         <v>-6.1</v>
       </c>
-      <c r="F61" s="1">
-        <v>1.5</v>
-      </c>
-      <c r="G61">
-        <v>-4.7</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>10</v>
       </c>
@@ -4255,16 +4299,18 @@
       </c>
       <c r="D62" s="1"/>
       <c r="E62">
-        <v>-6.1</v>
+        <f t="shared" si="7"/>
+        <v>-18.299999999999997</v>
       </c>
       <c r="F62" s="1">
         <v>1.5</v>
       </c>
       <c r="G62">
-        <v>-4.7</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+        <f>E62-E61</f>
+        <v>-6.0999999999999979</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>10</v>
       </c>
@@ -4276,31 +4322,26 @@
       </c>
       <c r="D63" s="1"/>
       <c r="E63">
-        <v>-6.1</v>
+        <f t="shared" si="7"/>
+        <v>-24.4</v>
       </c>
       <c r="F63" s="1">
         <v>1.5</v>
       </c>
       <c r="G63">
-        <v>-4.7</v>
+        <f>E63-E62</f>
+        <v>-6.1000000000000014</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:F63" xr:uid="{8156AB9F-69E8-A840-8709-7911BA63A67A}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="Global warming level"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="2">
-      <filters>
-        <filter val="Region"/>
-      </filters>
-    </filterColumn>
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F63">
       <sortCondition ref="A1:A63"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="E4 E7 G5:G6" formula="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>